<commit_message>
Updated marker ADTs and genes
</commit_message>
<xml_diff>
--- a/data/cluster_annotations/marker_proteins_macrophages_supp.xlsx
+++ b/data/cluster_annotations/marker_proteins_macrophages_supp.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maksimovicjovana/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7B7B94-577B-694E-BF2E-D6FCBB1764C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E4AD2F-22D3-E146-9CFC-676CFC35CAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="2280" windowWidth="26840" windowHeight="15940" xr2:uid="{4B227943-1172-2946-B9CB-103A9DF0C1CD}"/>
+    <workbookView xWindow="2260" yWindow="2260" windowWidth="26840" windowHeight="15940" xr2:uid="{4B227943-1172-2946-B9CB-103A9DF0C1CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="macrophages" sheetId="1" r:id="rId1"/>
+    <sheet name="macrophages" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">macrophages!$A$1:$A$34</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="225">
   <si>
     <t>HLADR</t>
   </si>
@@ -140,14 +140,587 @@
     <t>ADT</t>
   </si>
   <si>
-    <t>CD172a (SIRPα)</t>
+    <t>HLA-DRA</t>
+  </si>
+  <si>
+    <t>ENSG00000204287</t>
+  </si>
+  <si>
+    <t>AATAGCGAGCAAGTA</t>
+  </si>
+  <si>
+    <t>L243</t>
+  </si>
+  <si>
+    <t>anti-human HLA-DR</t>
+  </si>
+  <si>
+    <t>A0159</t>
+  </si>
+  <si>
+    <t>ENSG00000172322</t>
+  </si>
+  <si>
+    <t>CATTAGAGTCTGCCA</t>
+  </si>
+  <si>
+    <t>50C1</t>
+  </si>
+  <si>
+    <t>anti-human CLEC12A</t>
+  </si>
+  <si>
+    <t>A0853</t>
+  </si>
+  <si>
+    <t>ENSG00000010278</t>
+  </si>
+  <si>
+    <t>GAGTCACCAATCTGC</t>
+  </si>
+  <si>
+    <t>HI9a</t>
+  </si>
+  <si>
+    <t>anti-human CD9</t>
+  </si>
+  <si>
+    <t>A0579</t>
+  </si>
+  <si>
+    <t>ENSG00000114013</t>
+  </si>
+  <si>
+    <t>GTCTTTGTCAGTGCA</t>
+  </si>
+  <si>
+    <t>IT2.2</t>
+  </si>
+  <si>
+    <t>anti-human CD86</t>
+  </si>
+  <si>
+    <t>A0006</t>
+  </si>
+  <si>
+    <t>CD8A</t>
+  </si>
+  <si>
+    <t>ENSG00000153563</t>
+  </si>
+  <si>
+    <t>GCGCAACTTGATGAT</t>
+  </si>
+  <si>
+    <t>SK1</t>
+  </si>
+  <si>
+    <t>anti-human CD8</t>
+  </si>
+  <si>
+    <t>A0046</t>
+  </si>
+  <si>
+    <t>ENSG00000137101</t>
+  </si>
+  <si>
+    <t>CAGTCGTGGTAGATA</t>
+  </si>
+  <si>
+    <t>3F3</t>
+  </si>
+  <si>
+    <t>anti-human CD72</t>
+  </si>
+  <si>
+    <t>A0419</t>
+  </si>
+  <si>
+    <t>TFRC</t>
+  </si>
+  <si>
+    <t>ENSG00000072274</t>
+  </si>
+  <si>
+    <t>CCGTGTTCCTCATTA</t>
+  </si>
+  <si>
+    <t>CY1G4</t>
+  </si>
+  <si>
+    <t>anti-human CD71</t>
+  </si>
+  <si>
+    <t>A0394</t>
+  </si>
+  <si>
+    <t>ENSG00000173762</t>
+  </si>
+  <si>
+    <t>TGGATTCCCGGACTT</t>
+  </si>
+  <si>
+    <t>CD7-6B7</t>
+  </si>
+  <si>
+    <t>anti-human CD7</t>
+  </si>
+  <si>
+    <t>A0066</t>
+  </si>
+  <si>
+    <t>ENSG00000110848</t>
+  </si>
+  <si>
+    <t>GTCTCTTGGCTTAAA</t>
+  </si>
+  <si>
+    <t>FN50</t>
+  </si>
+  <si>
+    <t>anti-human CD69</t>
+  </si>
+  <si>
+    <t>A0146</t>
+  </si>
+  <si>
+    <t>ENSG00000135404</t>
+  </si>
+  <si>
+    <t>GAGATGTCTGCAACT</t>
+  </si>
+  <si>
+    <t>H5C6</t>
+  </si>
+  <si>
+    <t>anti-human CD63</t>
+  </si>
+  <si>
+    <t>A0404</t>
+  </si>
+  <si>
+    <t>ICAM1</t>
+  </si>
+  <si>
+    <t>ENSG00000090339</t>
+  </si>
+  <si>
+    <t>CTGATAGACTTGAGT</t>
+  </si>
+  <si>
+    <t>HA58</t>
+  </si>
+  <si>
+    <t>anti-human CD54</t>
+  </si>
+  <si>
+    <t>A0217</t>
+  </si>
+  <si>
+    <t>ENSG00000110448</t>
+  </si>
+  <si>
+    <t>CATTAACGGGATGCC</t>
+  </si>
+  <si>
+    <t>UCHT2</t>
+  </si>
+  <si>
+    <t>anti-human CD5</t>
+  </si>
+  <si>
+    <t>A0138</t>
+  </si>
+  <si>
+    <t>ENSG00000117091</t>
+  </si>
+  <si>
+    <t>CTACGACGTAGAAGA</t>
+  </si>
+  <si>
+    <t>BJ40</t>
+  </si>
+  <si>
+    <t>anti-human CD48</t>
+  </si>
+  <si>
+    <t>A0029</t>
+  </si>
+  <si>
+    <t>ENSG00000010610</t>
+  </si>
+  <si>
+    <t>TGTTCCCGCTCAACT</t>
+  </si>
+  <si>
+    <t>RPA-T4</t>
+  </si>
+  <si>
+    <t>anti-human CD4</t>
+  </si>
+  <si>
+    <t>A0072</t>
+  </si>
+  <si>
+    <t>FCGR2A</t>
+  </si>
+  <si>
+    <t>ENSG00000143226</t>
+  </si>
+  <si>
+    <t>GCTTCCGAATTACCG</t>
+  </si>
+  <si>
+    <t>FUN-2</t>
+  </si>
+  <si>
+    <t>anti-human CD32</t>
+  </si>
+  <si>
+    <t>A0142</t>
+  </si>
+  <si>
+    <t>PECAM1</t>
+  </si>
+  <si>
+    <t>ENSG00000261371</t>
+  </si>
+  <si>
+    <t>ACCTTTATGCCACGG</t>
+  </si>
+  <si>
+    <t>WM59</t>
+  </si>
+  <si>
+    <t>anti-human CD31</t>
+  </si>
+  <si>
+    <t>A0124</t>
+  </si>
+  <si>
+    <t>NRP1</t>
+  </si>
+  <si>
+    <t>ENSG00000099250</t>
+  </si>
+  <si>
+    <t>GGACTAAGTTTCGTT</t>
+  </si>
+  <si>
+    <t>12C2</t>
+  </si>
+  <si>
+    <t>anti-human CD304 (Neuropilin-1)</t>
+  </si>
+  <si>
+    <t>A0406</t>
+  </si>
+  <si>
+    <t>CD3D</t>
+  </si>
+  <si>
+    <t>ENSG00000167286</t>
+  </si>
+  <si>
+    <t>CTCATTGTAACTCCT</t>
+  </si>
+  <si>
+    <t>UCHT1</t>
+  </si>
+  <si>
+    <t>anti-human CD3</t>
+  </si>
+  <si>
+    <t>A0034</t>
+  </si>
+  <si>
+    <t>ENSG00000116824</t>
+  </si>
+  <si>
+    <t>TACGATTTGTCAGGG</t>
+  </si>
+  <si>
+    <t>TS1/8</t>
+  </si>
+  <si>
+    <t>anti-human CD2</t>
+  </si>
+  <si>
+    <t>A0367</t>
+  </si>
+  <si>
+    <t>SIRPA</t>
+  </si>
+  <si>
+    <t>ENSG00000198053</t>
+  </si>
+  <si>
+    <t>CGTGTTTAACTTGAG</t>
+  </si>
+  <si>
+    <t>15-414</t>
+  </si>
+  <si>
+    <t>anti-human CD172a (SIRPα)</t>
+  </si>
+  <si>
+    <t>A0408</t>
+  </si>
+  <si>
+    <t>CD172a</t>
+  </si>
+  <si>
+    <t>SIGLEC1</t>
+  </si>
+  <si>
+    <t>ENSG00000088827</t>
+  </si>
+  <si>
+    <t>TACTCAGCGTGTTTG</t>
+  </si>
+  <si>
+    <t>7-239</t>
+  </si>
+  <si>
+    <t>A0206</t>
+  </si>
+  <si>
+    <t>FCGR3A</t>
+  </si>
+  <si>
+    <t>ENSG00000203747</t>
+  </si>
+  <si>
+    <t>AAGTTCACTCTTTGC</t>
+  </si>
+  <si>
+    <t>3G8</t>
+  </si>
+  <si>
+    <t>anti-human CD16</t>
+  </si>
+  <si>
+    <t>A0083</t>
+  </si>
+  <si>
+    <t>PVR</t>
+  </si>
+  <si>
+    <t>ENSG00000073008</t>
+  </si>
+  <si>
+    <t>ATCACATCGTTGCCA</t>
+  </si>
+  <si>
+    <t>SKII.4</t>
+  </si>
+  <si>
+    <t>anti-human CD155 (PVR)</t>
+  </si>
+  <si>
+    <t>A0023</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>ENSG00000117525</t>
+  </si>
+  <si>
+    <t>CACTGCCGTCGATTA</t>
+  </si>
+  <si>
+    <t>NY2</t>
+  </si>
+  <si>
+    <t>anti-human CD142</t>
+  </si>
+  <si>
+    <t>A0822</t>
+  </si>
+  <si>
+    <t>THBD</t>
+  </si>
+  <si>
+    <t>ENSG00000178726</t>
+  </si>
+  <si>
+    <t>GGATAACCGCGCTTT</t>
+  </si>
+  <si>
+    <t>M80</t>
+  </si>
+  <si>
+    <t>anti-human CD141 (Thrombomodulin)</t>
+  </si>
+  <si>
+    <t>A0163</t>
+  </si>
+  <si>
+    <t>ENSG00000170458</t>
+  </si>
+  <si>
+    <t>TCTCAGACCTCCGTA</t>
+  </si>
+  <si>
+    <t>M5E2</t>
+  </si>
+  <si>
+    <t>anti-human CD14</t>
+  </si>
+  <si>
+    <t>A0081</t>
+  </si>
+  <si>
+    <t>ANPEP</t>
+  </si>
+  <si>
+    <t>ENSG00000166825</t>
+  </si>
+  <si>
+    <t>TTTCAACGCCCTTTC</t>
+  </si>
+  <si>
+    <t>WM15</t>
+  </si>
+  <si>
+    <t>anti-human CD13</t>
+  </si>
+  <si>
+    <t>A0364</t>
+  </si>
+  <si>
+    <t>IL3RA</t>
+  </si>
+  <si>
+    <t>ENSG00000185291</t>
+  </si>
+  <si>
+    <t>CTTCACTCTGTCAGG</t>
+  </si>
+  <si>
+    <t>6H6</t>
+  </si>
+  <si>
+    <t>anti-human CD123</t>
+  </si>
+  <si>
+    <t>A0064</t>
+  </si>
+  <si>
+    <t>ITGAX</t>
+  </si>
+  <si>
+    <t>ENSG00000140678</t>
+  </si>
+  <si>
+    <t>TACGCCTATAACTTG</t>
+  </si>
+  <si>
+    <t>S-HCL-3</t>
+  </si>
+  <si>
+    <t>anti-human CD11c</t>
+  </si>
+  <si>
+    <t>A0053</t>
+  </si>
+  <si>
+    <t>ITGAM</t>
+  </si>
+  <si>
+    <t>ENSG00000169896</t>
+  </si>
+  <si>
+    <t>GACAAGTGATCTGCA</t>
+  </si>
+  <si>
+    <t>ICRF44</t>
+  </si>
+  <si>
+    <t>anti-human CD11b</t>
+  </si>
+  <si>
+    <t>A0161</t>
+  </si>
+  <si>
+    <t>LAMP1</t>
+  </si>
+  <si>
+    <t>ENSG00000185896</t>
+  </si>
+  <si>
+    <t>CAGCCCACTGCAATA</t>
+  </si>
+  <si>
+    <t>H4A3</t>
+  </si>
+  <si>
+    <t>anti-human CD107a (LAMP-1)</t>
+  </si>
+  <si>
+    <t>A0155</t>
+  </si>
+  <si>
+    <t>ITGAE</t>
+  </si>
+  <si>
+    <t>ENSG00000083457</t>
+  </si>
+  <si>
+    <t>GACCTCATTGTGAAT</t>
+  </si>
+  <si>
+    <t>Ber-ACT8</t>
+  </si>
+  <si>
+    <t>Hu CD103 (Integrin αE)</t>
+  </si>
+  <si>
+    <t>A0145</t>
+  </si>
+  <si>
+    <t>ENSG00000134256</t>
+  </si>
+  <si>
+    <t>CTACTTCCCTGTCAA</t>
+  </si>
+  <si>
+    <t>BB27</t>
+  </si>
+  <si>
+    <t>anti-human CD101 (BB27)</t>
+  </si>
+  <si>
+    <t>A0944</t>
+  </si>
+  <si>
+    <t>Gene Name</t>
+  </si>
+  <si>
+    <t>Ensembl ID</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Clone</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>DNA_ID</t>
+  </si>
+  <si>
+    <t>anti-human CD169 (Sialoadhesin; Siglec-1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +736,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,7 +764,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -180,13 +772,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,183 +1225,804 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDDC629-81D1-DD49-A40F-25C5B424A133}">
-  <dimension ref="A1:A34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF56E063-A463-4D4A-96BB-DF4658FA8623}">
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>